<commit_message>
Verwijderen van 'p.p.' uit was-wordt VvN codes
</commit_message>
<xml_diff>
--- a/data/ww_split.xlsx
+++ b/data/ww_split.xlsx
@@ -15540,7 +15540,7 @@
       </c>
       <c r="B622" t="inlineStr">
         <is>
-          <t>20Aa01ap.p.</t>
+          <t>20Aa01a</t>
         </is>
       </c>
       <c r="C622" t="inlineStr">
@@ -15852,7 +15852,7 @@
       </c>
       <c r="B634" t="inlineStr">
         <is>
-          <t>11RG02p.p.</t>
+          <t>11RG02</t>
         </is>
       </c>
       <c r="C634" t="inlineStr">

</xml_diff>